<commit_message>
Included Walkingdistances/Terminal Preferences, first real results!
</commit_message>
<xml_diff>
--- a/Inputs/WalkingDistances.xlsx
+++ b/Inputs/WalkingDistances.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pavel\Documents\Git\Operations\GateAndBayAssignment\Scripts\Inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hyperion\Documents\Personal Documents\Coding\GateAndBayAssignment\Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{969EF30C-131B-48F6-97E8-E8569AB8D79D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{013C2782-26DE-45CE-8687-7DDE3572E65E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000" xr2:uid="{27EC7086-3171-4A61-AF29-E40EE245423A}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>Terminal</t>
   </si>
@@ -154,13 +154,25 @@
   </si>
   <si>
     <t>D2A</t>
+  </si>
+  <si>
+    <t>H7</t>
+  </si>
+  <si>
+    <t>H8</t>
+  </si>
+  <si>
+    <t>H9</t>
+  </si>
+  <si>
+    <t>H10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -172,13 +184,6 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Utopia-Regular"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -216,16 +221,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -549,15 +550,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{978EA0CE-BA00-416E-AB96-A86200477523}">
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -586,7 +587,7 @@
       <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="4">
         <v>2</v>
       </c>
       <c r="C3" s="1">
@@ -603,7 +604,7 @@
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="4">
         <v>3</v>
       </c>
       <c r="C4" s="1">
@@ -620,7 +621,7 @@
       <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="4">
         <v>4</v>
       </c>
       <c r="C5" s="1">
@@ -637,7 +638,7 @@
       <c r="A6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="4">
         <v>3</v>
       </c>
       <c r="C6" s="1">
@@ -654,7 +655,7 @@
       <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="4">
         <v>0</v>
       </c>
       <c r="C7" s="1">
@@ -671,7 +672,7 @@
       <c r="A8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="4">
         <v>5</v>
       </c>
       <c r="C8" s="1">
@@ -688,7 +689,7 @@
       <c r="A9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="4">
         <v>6</v>
       </c>
       <c r="C9" s="1">
@@ -705,7 +706,7 @@
       <c r="A10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="4">
         <v>7</v>
       </c>
       <c r="C10" s="1">
@@ -725,7 +726,7 @@
       <c r="B11" s="1">
         <v>8</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="4">
         <v>6</v>
       </c>
       <c r="D11" s="1">
@@ -742,7 +743,7 @@
       <c r="B12" s="1">
         <v>9</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="4">
         <v>5</v>
       </c>
       <c r="D12" s="1">
@@ -759,7 +760,7 @@
       <c r="B13" s="1">
         <v>10</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="4">
         <v>4</v>
       </c>
       <c r="D13" s="1">
@@ -776,7 +777,7 @@
       <c r="B14" s="1">
         <v>11</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="4">
         <v>3</v>
       </c>
       <c r="D14" s="1">
@@ -793,7 +794,7 @@
       <c r="B15" s="1">
         <v>12</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="4">
         <v>2</v>
       </c>
       <c r="D15" s="1">
@@ -813,7 +814,7 @@
       <c r="C16" s="1">
         <v>1</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D16" s="4">
         <v>2</v>
       </c>
       <c r="E16" s="1">
@@ -830,7 +831,7 @@
       <c r="C17" s="1">
         <v>0</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D17" s="4">
         <v>1</v>
       </c>
       <c r="E17" s="1">
@@ -847,7 +848,7 @@
       <c r="C18" s="1">
         <v>2</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D18" s="4">
         <v>0</v>
       </c>
       <c r="E18" s="1">
@@ -867,7 +868,7 @@
       <c r="D19" s="1">
         <v>3</v>
       </c>
-      <c r="E19" s="6">
+      <c r="E19" s="4">
         <v>2</v>
       </c>
     </row>
@@ -884,7 +885,7 @@
       <c r="D20" s="1">
         <v>2</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E20" s="4">
         <v>1</v>
       </c>
     </row>
@@ -901,7 +902,7 @@
       <c r="D21" s="1">
         <v>1</v>
       </c>
-      <c r="E21" s="6">
+      <c r="E21" s="4">
         <v>0</v>
       </c>
     </row>
@@ -918,7 +919,7 @@
       <c r="D22" s="1">
         <v>3</v>
       </c>
-      <c r="E22" s="6">
+      <c r="E22" s="4">
         <v>3</v>
       </c>
     </row>
@@ -935,24 +936,24 @@
       <c r="D23" s="1">
         <v>2</v>
       </c>
-      <c r="E23" s="6">
+      <c r="E23" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B24" s="5">
+      <c r="B24" s="3">
         <v>19</v>
       </c>
-      <c r="C24" s="5">
+      <c r="C24" s="3">
         <v>5</v>
       </c>
-      <c r="D24" s="5">
+      <c r="D24" s="3">
         <v>1</v>
       </c>
-      <c r="E24" s="7">
+      <c r="E24" s="5">
         <v>1</v>
       </c>
     </row>
@@ -1212,11 +1213,72 @@
       </c>
     </row>
     <row r="40" spans="1:5">
-      <c r="A40" s="3"/>
-      <c r="B40" s="4"/>
-      <c r="C40" s="4"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
+      <c r="A40" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B40" s="1">
+        <v>200</v>
+      </c>
+      <c r="C40" s="1">
+        <v>200</v>
+      </c>
+      <c r="D40" s="1">
+        <v>200</v>
+      </c>
+      <c r="E40" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B41" s="1">
+        <v>200</v>
+      </c>
+      <c r="C41" s="1">
+        <v>200</v>
+      </c>
+      <c r="D41" s="1">
+        <v>200</v>
+      </c>
+      <c r="E41" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B42" s="1">
+        <v>200</v>
+      </c>
+      <c r="C42" s="1">
+        <v>200</v>
+      </c>
+      <c r="D42" s="1">
+        <v>200</v>
+      </c>
+      <c r="E42" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B43" s="1">
+        <v>200</v>
+      </c>
+      <c r="C43" s="1">
+        <v>200</v>
+      </c>
+      <c r="D43" s="1">
+        <v>200</v>
+      </c>
+      <c r="E43" s="1">
+        <v>200</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>